<commit_message>
GUI improvments, update of excel template and better support for one source code file tests.
</commit_message>
<xml_diff>
--- a/excelTemplate/template.xlsx
+++ b/excelTemplate/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\JJudge\excelTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Projetos\Corretor de Exercícios\JJudge\excelTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29216C56-FCBA-40DE-9E08-980C6EBA8AFF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F52AB1-6546-4874-BA56-124AF2379875}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{CAE12B05-0ADD-4CDD-9C8A-3403F00F304E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{CAE12B05-0ADD-4CDD-9C8A-3403F00F304E}"/>
   </bookViews>
   <sheets>
     <sheet name="grades" sheetId="1" r:id="rId1"/>
@@ -26,25 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="20">
-  <si>
-    <t>A: approved</t>
-  </si>
-  <si>
-    <t>R: reproved</t>
-  </si>
-  <si>
-    <t>CE: compilation error</t>
-  </si>
-  <si>
-    <t>RE: runtime error</t>
-  </si>
-  <si>
-    <t>TE: timeout error</t>
-  </si>
-  <si>
-    <t>FE: file not found error</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>A</t>
   </si>
@@ -87,12 +69,18 @@
   <si>
     <t>file not found error</t>
   </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>don't check</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,14 +92,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFC000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -134,6 +114,46 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF7F27"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFA349A4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF5B00B7"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF787878"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -174,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -183,21 +203,184 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FFFF7F27"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FFA349A4"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF5B00B7"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF787878"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FFFF7F27"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FFA349A4"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF5B00B7"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF787878"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FFFF7F27"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FFFFC000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FFFFC000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FFFFC000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -248,6 +431,15 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF787878"/>
+      <color rgb="FF5B00B7"/>
+      <color rgb="FFA349A4"/>
+      <color rgb="FFFF7F27"/>
+      <color rgb="FF5EAEFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -558,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADDC85A9-572F-46E8-AFFE-0E8BF7B4FAB0}">
   <dimension ref="A1:BA61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3925,23 +4117,26 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:BA61">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>"FE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
       <formula>"TE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
       <formula>"RE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
       <formula>"CE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+      <formula>"DC"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -3951,10 +4146,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B164C38-FF2B-4C2E-9AD1-FF5FE2E8A917}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3965,58 +4160,66 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="3" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="7" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Applying i18n to missing artifacts.
</commit_message>
<xml_diff>
--- a/excelTemplate/template.xlsx
+++ b/excelTemplate/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Projetos\Corretor de Exercícios\JJudge\excelTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Projetos e Códigos\Corretor de Exercícios\JJudge\excelTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F52AB1-6546-4874-BA56-124AF2379875}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24DDC819-9A20-4917-9481-2434536E7CFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{CAE12B05-0ADD-4CDD-9C8A-3403F00F304E}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11505" xr2:uid="{CAE12B05-0ADD-4CDD-9C8A-3403F00F304E}"/>
   </bookViews>
   <sheets>
     <sheet name="grades" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>A</t>
   </si>
@@ -46,34 +46,7 @@
     <t>FE</t>
   </si>
   <si>
-    <t>label</t>
-  </si>
-  <si>
-    <t>meaning</t>
-  </si>
-  <si>
-    <t>approved</t>
-  </si>
-  <si>
-    <t>reproved</t>
-  </si>
-  <si>
-    <t>compilation error</t>
-  </si>
-  <si>
-    <t>runtime error</t>
-  </si>
-  <si>
-    <t>timeout error</t>
-  </si>
-  <si>
-    <t>file not found error</t>
-  </si>
-  <si>
     <t>DC</t>
-  </si>
-  <si>
-    <t>don't check</t>
   </si>
 </sst>
 </file>
@@ -229,55 +202,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color rgb="FFFF7F27"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color rgb="FFA349A4"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color rgb="FF5B00B7"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color rgb="FF787878"/>
-      </font>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <b/>
@@ -331,102 +256,6 @@
         <i val="0"/>
         <strike val="0"/>
         <color rgb="FF787878"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color rgb="FFFF7F27"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color rgb="FFFFC000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color rgb="FFFFC000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color rgb="FFFFC000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color rgb="FFFFC000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color rgb="FFFFC000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color rgb="FFFFC000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color rgb="FFFFC000"/>
       </font>
     </dxf>
   </dxfs>
@@ -750,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADDC85A9-572F-46E8-AFFE-0E8BF7B4FAB0}">
   <dimension ref="A1:BA61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="W10" sqref="W10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4117,25 +3946,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:BA61">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"FE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"TE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"RE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"CE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
       <formula>"A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"DC"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4149,78 +3978,60 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="B2" s="6"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>9</v>
-      </c>
+      <c r="B3" s="6"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="B4" s="6"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="B5" s="6"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="B6" s="6"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="B7" s="6"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="B8" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>